<commit_message>
Extract comments from the worksheets of a .xlsx file
</commit_message>
<xml_diff>
--- a/test/files/func_comment_drawing.xlsx
+++ b/test/files/func_comment_drawing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\purch\OneDrive\デスクトップ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE75EA84-7F6B-40F5-965C-7A56092C83E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBB8B3A-2639-4740-ADC2-BC764213EB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00C2C209-37A7-41F7-8C2F-38432223F584}"/>
   </bookViews>
@@ -37,19 +37,8 @@
     <author>黒田努</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{D014CA45-9A73-48D2-9CFA-7658FF8F9577}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{1E4DF852-5CA8-4A03-AA5E-77638F7411DC}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="MS P ゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>黒田努:</t>
-        </r>
         <r>
           <rPr>
             <sz val="9"/>
@@ -58,8 +47,35 @@
             <family val="3"/>
             <charset val="128"/>
           </rPr>
-          <t xml:space="preserve">
-Sum</t>
+          <t>Value 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{1C569291-E7F6-454E-B3FA-A767BD0EA233}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="MS P ゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Value 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{D014CA45-9A73-48D2-9CFA-7658FF8F9577}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="MS P ゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Sum</t>
         </r>
       </text>
     </comment>
@@ -86,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,14 +119,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="MS P ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="MS P ゴシック"/>
@@ -530,7 +538,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
Extract texts in drawings from Excel sheets
</commit_message>
<xml_diff>
--- a/test/files/func_comment_drawing.xlsx
+++ b/test/files/func_comment_drawing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\purch\OneDrive\デスクトップ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBB8B3A-2639-4740-ADC2-BC764213EB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9740763-0C75-4ED1-B932-EDB3D50A009D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00C2C209-37A7-41F7-8C2F-38432223F584}"/>
   </bookViews>
@@ -235,6 +235,70 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="楕円 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C1249AD-AE72-4684-BED6-B4B8722D8B5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4381500" y="1476375"/>
+          <a:ext cx="1295400" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Good job!</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -538,7 +602,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>